<commit_message>
Update Pool Connection & Promisify
</commit_message>
<xml_diff>
--- a/Alert_Report/2020-04-01.xlsx
+++ b/Alert_Report/2020-04-01.xlsx
@@ -393,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -409,7 +409,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>400</v>
+        <v>444</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -417,7 +417,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>401</v>
+        <v>445</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -425,7 +425,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>402</v>
+        <v>446</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -433,15 +433,7 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>404</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>